<commit_message>
fix: standarized surveillance yes no variable
</commit_message>
<xml_diff>
--- a/src/Data/country_data.xlsx
+++ b/src/Data/country_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D74919E-927A-2B4B-A3ED-294786412A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC335E5B-C45F-0D47-89B0-BD66DBC5AFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45980" yWindow="2780" windowWidth="30240" windowHeight="18880" xr2:uid="{7CFA64C4-648F-B840-901A-EC2D94882293}"/>
+    <workbookView xWindow="45980" yWindow="2780" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{7CFA64C4-648F-B840-901A-EC2D94882293}"/>
   </bookViews>
   <sheets>
     <sheet name="1-General" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7603" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7657" uniqueCount="448">
   <si>
     <t>Datos generales</t>
   </si>
@@ -1316,12 +1316,6 @@
     <t>USUMATLÁN</t>
   </si>
   <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>si</t>
   </si>
   <si>
@@ -1329,9 +1323,6 @@
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>Guatemala</t>
@@ -1395,6 +1386,9 @@
   </si>
   <si>
     <t>Esquema de vacunación contra el polio</t>
+  </si>
+  <si>
+    <t>Na</t>
   </si>
 </sst>
 </file>
@@ -2496,7 +2490,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18904028-F9F6-3046-9356-B730934F1CDF}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2516,7 +2512,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2537,7 +2533,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B5" s="2">
         <v>340</v>
@@ -2545,7 +2541,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B6" s="2"/>
     </row>
@@ -2590,10 +2586,10 @@
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>11</v>
@@ -2914,7 +2910,7 @@
         <v>85</v>
       </c>
       <c r="D18" s="48" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="E18" s="48"/>
       <c r="F18" s="48"/>
@@ -3921,7 +3917,7 @@
         <v>153</v>
       </c>
       <c r="D71" s="48" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E71" s="48"/>
       <c r="F71" s="48"/>
@@ -4358,7 +4354,7 @@
         <v>183</v>
       </c>
       <c r="D94" s="48" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E94" s="48"/>
       <c r="F94" s="48"/>
@@ -4624,7 +4620,7 @@
         <v>183</v>
       </c>
       <c r="D108" s="48" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="E108" s="48"/>
       <c r="F108" s="48"/>
@@ -4966,7 +4962,7 @@
         <v>213</v>
       </c>
       <c r="D126" s="48" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E126" s="48"/>
       <c r="F126" s="48"/>
@@ -5004,7 +5000,7 @@
         <v>213</v>
       </c>
       <c r="D128" s="48" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E128" s="48"/>
       <c r="F128" s="48"/>
@@ -5954,7 +5950,7 @@
         <v>258</v>
       </c>
       <c r="D178" s="48" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="E178" s="48"/>
       <c r="F178" s="48"/>
@@ -6087,7 +6083,7 @@
         <v>258</v>
       </c>
       <c r="D185" s="48" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="E185" s="48"/>
       <c r="F185" s="48"/>
@@ -6372,7 +6368,7 @@
         <v>213</v>
       </c>
       <c r="D200" s="48" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="E200" s="48"/>
       <c r="F200" s="48"/>
@@ -6733,7 +6729,7 @@
         <v>296</v>
       </c>
       <c r="D219" s="48" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="E219" s="48"/>
       <c r="F219" s="48"/>
@@ -6809,7 +6805,7 @@
         <v>304</v>
       </c>
       <c r="D223" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="E223" s="48"/>
       <c r="F223" s="48"/>
@@ -7208,7 +7204,7 @@
         <v>320</v>
       </c>
       <c r="D244" s="48" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="E244" s="48"/>
       <c r="F244" s="48"/>
@@ -9068,8 +9064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87362FD8-F1C8-0142-963D-AD6273C5898D}">
   <dimension ref="A1:O342"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9097,10 +9093,10 @@
         <v>10</v>
       </c>
       <c r="E1" s="55" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="F1" s="55" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G1" s="55" t="s">
         <v>11</v>
@@ -9848,7 +9844,7 @@
         <v>85</v>
       </c>
       <c r="D19" s="48" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="E19" s="48"/>
       <c r="F19" s="48"/>
@@ -12127,7 +12123,7 @@
         <v>153</v>
       </c>
       <c r="D72" s="48" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E72" s="48"/>
       <c r="F72" s="48"/>
@@ -12350,7 +12346,7 @@
         <v>279727</v>
       </c>
       <c r="H77" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I77">
         <v>73.893505991495942</v>
@@ -12436,7 +12432,7 @@
         <v>124548</v>
       </c>
       <c r="H79" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I79">
         <v>74.493299368700846</v>
@@ -13038,7 +13034,7 @@
         <v>130776</v>
       </c>
       <c r="H93" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I93">
         <v>76.350048216007721</v>
@@ -13116,7 +13112,7 @@
         <v>183</v>
       </c>
       <c r="D95" s="48" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E95" s="48"/>
       <c r="F95" s="48"/>
@@ -13718,7 +13714,7 @@
         <v>183</v>
       </c>
       <c r="D109" s="48" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="E109" s="48"/>
       <c r="F109" s="48"/>
@@ -14492,7 +14488,7 @@
         <v>213</v>
       </c>
       <c r="D127" s="48" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E127" s="48"/>
       <c r="F127" s="48"/>
@@ -14578,7 +14574,7 @@
         <v>213</v>
       </c>
       <c r="D129" s="48" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E129" s="48"/>
       <c r="F129" s="48"/>
@@ -15940,7 +15936,7 @@
         <v>175.1</v>
       </c>
       <c r="O160" s="49" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="161" spans="1:15" x14ac:dyDescent="0.2">
@@ -16728,7 +16724,7 @@
         <v>258</v>
       </c>
       <c r="D179" s="48" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="E179" s="48"/>
       <c r="F179" s="48"/>
@@ -16757,7 +16753,7 @@
         <v>87.2</v>
       </c>
       <c r="O179" s="49" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.2">
@@ -17029,7 +17025,7 @@
         <v>258</v>
       </c>
       <c r="D186" s="48" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="E186" s="48"/>
       <c r="F186" s="48"/>
@@ -17674,7 +17670,7 @@
         <v>213</v>
       </c>
       <c r="D201" s="48" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="E201" s="48"/>
       <c r="F201" s="48"/>
@@ -18047,7 +18043,7 @@
         <v>91.4</v>
       </c>
       <c r="O209" s="49" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="210" spans="1:15" x14ac:dyDescent="0.2">
@@ -18090,7 +18086,7 @@
         <v>87.7</v>
       </c>
       <c r="O210" s="49" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="211" spans="1:15" x14ac:dyDescent="0.2">
@@ -18491,7 +18487,7 @@
         <v>296</v>
       </c>
       <c r="D220" s="48" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="E220" s="48"/>
       <c r="F220" s="48"/>
@@ -18563,7 +18559,7 @@
         <v>100.4</v>
       </c>
       <c r="O221" s="49" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="222" spans="1:15" x14ac:dyDescent="0.2">
@@ -18663,7 +18659,7 @@
         <v>304</v>
       </c>
       <c r="D224" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="E224" s="48"/>
       <c r="F224" s="48"/>
@@ -19566,7 +19562,7 @@
         <v>320</v>
       </c>
       <c r="D245" s="48" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="E245" s="48"/>
       <c r="F245" s="48"/>
@@ -20238,7 +20234,7 @@
         <v>98</v>
       </c>
       <c r="O260" s="49" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="261" spans="1:15" x14ac:dyDescent="0.2">
@@ -20324,7 +20320,7 @@
         <v>97</v>
       </c>
       <c r="O262" s="49" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="263" spans="1:15" x14ac:dyDescent="0.2">
@@ -20711,7 +20707,7 @@
         <v>108</v>
       </c>
       <c r="O271" s="49" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="272" spans="1:15" x14ac:dyDescent="0.2">
@@ -23795,8 +23791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24FC60A-8114-B04C-B5D4-941061AFF1F9}">
   <dimension ref="A1:O342"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23825,10 +23821,10 @@
         <v>10</v>
       </c>
       <c r="E1" s="55" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="F1" s="55" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G1" s="55" t="s">
         <v>11</v>
@@ -23921,7 +23917,7 @@
         <v>0</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>428</v>
+        <v>447</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -23954,7 +23950,7 @@
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -23987,7 +23983,7 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -24029,7 +24025,9 @@
       <c r="N6" s="5">
         <v>0</v>
       </c>
-      <c r="O6" s="5"/>
+      <c r="O6" s="5" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -24061,7 +24059,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -24094,7 +24092,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -24124,7 +24122,7 @@
       <c r="J9" s="49"/>
       <c r="K9" s="49"/>
       <c r="O9" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -24154,7 +24152,7 @@
       <c r="J10" s="49"/>
       <c r="K10" s="49"/>
       <c r="O10" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -24184,7 +24182,7 @@
       <c r="J11" s="49"/>
       <c r="K11" s="49"/>
       <c r="O11" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -24226,7 +24224,9 @@
       <c r="N12">
         <v>100</v>
       </c>
-      <c r="O12" s="49"/>
+      <c r="O12" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -24255,7 +24255,7 @@
       <c r="J13" s="49"/>
       <c r="K13" s="49"/>
       <c r="O13" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -24285,7 +24285,7 @@
       <c r="J14" s="49"/>
       <c r="K14" s="49"/>
       <c r="O14" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -24315,7 +24315,7 @@
       <c r="J15" s="49"/>
       <c r="K15" s="49"/>
       <c r="O15" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -24345,7 +24345,7 @@
       <c r="J16" s="49"/>
       <c r="K16" s="49"/>
       <c r="O16" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -24387,7 +24387,9 @@
       <c r="N17">
         <v>0</v>
       </c>
-      <c r="O17" s="49"/>
+      <c r="O17" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -24416,7 +24418,7 @@
       <c r="J18" s="49"/>
       <c r="K18" s="49"/>
       <c r="O18" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
@@ -24430,7 +24432,7 @@
         <v>85</v>
       </c>
       <c r="D19" s="48" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="E19" s="48"/>
       <c r="F19" s="48"/>
@@ -24446,7 +24448,7 @@
       <c r="J19" s="49"/>
       <c r="K19" s="49"/>
       <c r="O19" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -24476,7 +24478,7 @@
       <c r="J20" s="49"/>
       <c r="K20" s="49"/>
       <c r="O20" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -24506,7 +24508,7 @@
       <c r="J21" s="49"/>
       <c r="K21" s="49"/>
       <c r="O21" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -24536,7 +24538,7 @@
       <c r="J22" s="49"/>
       <c r="K22" s="49"/>
       <c r="O22" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
@@ -24566,7 +24568,7 @@
       <c r="J23" s="49"/>
       <c r="K23" s="49"/>
       <c r="O23" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -24596,7 +24598,7 @@
       <c r="J24" s="49"/>
       <c r="K24" s="49"/>
       <c r="O24" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
@@ -24626,7 +24628,7 @@
       <c r="J25" s="49"/>
       <c r="K25" s="49"/>
       <c r="O25" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -24656,7 +24658,7 @@
       <c r="J26" s="49"/>
       <c r="K26" s="49"/>
       <c r="O26" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
@@ -24686,7 +24688,7 @@
       <c r="J27" s="49"/>
       <c r="K27" s="49"/>
       <c r="O27" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
@@ -24716,7 +24718,7 @@
       <c r="J28" s="49"/>
       <c r="K28" s="49"/>
       <c r="O28" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -24746,7 +24748,7 @@
       <c r="J29" s="49"/>
       <c r="K29" s="49"/>
       <c r="O29" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
@@ -24776,7 +24778,7 @@
       <c r="J30" s="49"/>
       <c r="K30" s="49"/>
       <c r="O30" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
@@ -24806,7 +24808,7 @@
       <c r="J31" s="49"/>
       <c r="K31" s="49"/>
       <c r="O31" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -24836,7 +24838,7 @@
       <c r="J32" s="49"/>
       <c r="K32" s="49"/>
       <c r="O32" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
@@ -24878,7 +24880,9 @@
       <c r="N33">
         <v>0</v>
       </c>
-      <c r="O33" s="49"/>
+      <c r="O33" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34">
@@ -24907,7 +24911,7 @@
       <c r="J34" s="49"/>
       <c r="K34" s="49"/>
       <c r="O34" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
@@ -24937,7 +24941,7 @@
       <c r="J35" s="49"/>
       <c r="K35" s="49"/>
       <c r="O35" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
@@ -24967,7 +24971,7 @@
       <c r="J36" s="49"/>
       <c r="K36" s="49"/>
       <c r="O36" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
@@ -24997,7 +25001,7 @@
       <c r="J37" s="49"/>
       <c r="K37" s="49"/>
       <c r="O37" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
@@ -25027,7 +25031,7 @@
       <c r="J38" s="49"/>
       <c r="K38" s="49"/>
       <c r="O38" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
@@ -25057,7 +25061,7 @@
       <c r="J39" s="49"/>
       <c r="K39" s="49"/>
       <c r="O39" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
@@ -25087,7 +25091,7 @@
       <c r="J40" s="49"/>
       <c r="K40" s="49"/>
       <c r="O40" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
@@ -25129,7 +25133,9 @@
       <c r="N41">
         <v>50</v>
       </c>
-      <c r="O41" s="49"/>
+      <c r="O41" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42">
@@ -25158,7 +25164,7 @@
       <c r="J42" s="49"/>
       <c r="K42" s="49"/>
       <c r="O42" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -25188,7 +25194,7 @@
       <c r="J43" s="49"/>
       <c r="K43" s="49"/>
       <c r="O43" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -25230,7 +25236,9 @@
       <c r="N44">
         <v>100</v>
       </c>
-      <c r="O44" s="49"/>
+      <c r="O44" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45">
@@ -25259,7 +25267,7 @@
       <c r="J45" s="49"/>
       <c r="K45" s="49"/>
       <c r="O45" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
@@ -25289,7 +25297,7 @@
       <c r="J46" s="49"/>
       <c r="K46" s="49"/>
       <c r="O46" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
@@ -25319,7 +25327,7 @@
       <c r="J47" s="49"/>
       <c r="K47" s="49"/>
       <c r="O47" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
@@ -25349,7 +25357,7 @@
       <c r="J48" s="49"/>
       <c r="K48" s="49"/>
       <c r="O48" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
@@ -25379,7 +25387,7 @@
       <c r="J49" s="49"/>
       <c r="K49" s="49"/>
       <c r="O49" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
@@ -25421,7 +25429,9 @@
       <c r="N50">
         <v>100</v>
       </c>
-      <c r="O50" s="49"/>
+      <c r="O50" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51">
@@ -25450,7 +25460,7 @@
       <c r="J51" s="49"/>
       <c r="K51" s="49"/>
       <c r="O51" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
@@ -25480,7 +25490,7 @@
       <c r="J52" s="49"/>
       <c r="K52" s="49"/>
       <c r="O52" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
@@ -25522,7 +25532,9 @@
       <c r="N53">
         <v>100</v>
       </c>
-      <c r="O53" s="49"/>
+      <c r="O53" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54">
@@ -25551,7 +25563,7 @@
       <c r="J54" s="49"/>
       <c r="K54" s="49"/>
       <c r="O54" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
@@ -25581,7 +25593,7 @@
       <c r="J55" s="49"/>
       <c r="K55" s="49"/>
       <c r="O55" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
@@ -25611,7 +25623,7 @@
       <c r="J56" s="49"/>
       <c r="K56" s="49"/>
       <c r="O56" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
@@ -25641,7 +25653,7 @@
       <c r="J57" s="49"/>
       <c r="K57" s="49"/>
       <c r="O57" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
@@ -25683,7 +25695,9 @@
       <c r="N58">
         <v>0</v>
       </c>
-      <c r="O58" s="49"/>
+      <c r="O58" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59">
@@ -25712,7 +25726,7 @@
       <c r="J59" s="49"/>
       <c r="K59" s="49"/>
       <c r="O59" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
@@ -25742,7 +25756,7 @@
       <c r="J60" s="49"/>
       <c r="K60" s="49"/>
       <c r="O60" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
@@ -25772,7 +25786,7 @@
       <c r="J61" s="49"/>
       <c r="K61" s="49"/>
       <c r="O61" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
@@ -25802,7 +25816,7 @@
       <c r="J62" s="49"/>
       <c r="K62" s="49"/>
       <c r="O62" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
@@ -25844,7 +25858,9 @@
       <c r="N63">
         <v>50</v>
       </c>
-      <c r="O63" s="49"/>
+      <c r="O63" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64">
@@ -25873,7 +25889,7 @@
       <c r="J64" s="49"/>
       <c r="K64" s="49"/>
       <c r="O64" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
@@ -25903,7 +25919,7 @@
       <c r="J65" s="49"/>
       <c r="K65" s="49"/>
       <c r="O65" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
@@ -25933,7 +25949,7 @@
       <c r="J66" s="49"/>
       <c r="K66" s="49"/>
       <c r="O66" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
@@ -25963,7 +25979,7 @@
       <c r="J67" s="49"/>
       <c r="K67" s="49"/>
       <c r="O67" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
@@ -25993,7 +26009,7 @@
       <c r="J68" s="49"/>
       <c r="K68" s="49"/>
       <c r="O68" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
@@ -26023,7 +26039,7 @@
       <c r="J69" s="49"/>
       <c r="K69" s="49"/>
       <c r="O69" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.2">
@@ -26053,7 +26069,7 @@
       <c r="J70" s="49"/>
       <c r="K70" s="49"/>
       <c r="O70" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.2">
@@ -26083,7 +26099,7 @@
       <c r="J71" s="49"/>
       <c r="K71" s="49"/>
       <c r="O71" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.2">
@@ -26097,7 +26113,7 @@
         <v>153</v>
       </c>
       <c r="D72" s="48" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E72" s="48"/>
       <c r="F72" s="48"/>
@@ -26113,7 +26129,7 @@
       <c r="J72" s="49"/>
       <c r="K72" s="49"/>
       <c r="O72" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
@@ -26143,7 +26159,7 @@
       <c r="J73" s="49"/>
       <c r="K73" s="49"/>
       <c r="O73" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
@@ -26173,7 +26189,7 @@
       <c r="J74" s="49"/>
       <c r="K74" s="49"/>
       <c r="O74" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.2">
@@ -26203,7 +26219,7 @@
       <c r="J75" s="49"/>
       <c r="K75" s="49"/>
       <c r="O75" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.2">
@@ -26233,7 +26249,7 @@
       <c r="J76" s="49"/>
       <c r="K76" s="49"/>
       <c r="O76" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.2">
@@ -26255,7 +26271,7 @@
         <v>279727</v>
       </c>
       <c r="H77" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I77" s="51">
         <v>79</v>
@@ -26275,7 +26291,9 @@
       <c r="N77">
         <v>0</v>
       </c>
-      <c r="O77" s="49"/>
+      <c r="O77" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78">
@@ -26304,7 +26322,7 @@
       <c r="J78" s="49"/>
       <c r="K78" s="49"/>
       <c r="O78" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.2">
@@ -26326,7 +26344,7 @@
         <v>124548</v>
       </c>
       <c r="H79" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I79" s="51">
         <v>75</v>
@@ -26346,7 +26364,9 @@
       <c r="N79">
         <v>0</v>
       </c>
-      <c r="O79" s="49"/>
+      <c r="O79" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80">
@@ -26375,7 +26395,7 @@
       <c r="J80" s="49"/>
       <c r="K80" s="49"/>
       <c r="O80" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.2">
@@ -26405,7 +26425,7 @@
       <c r="J81" s="49"/>
       <c r="K81" s="49"/>
       <c r="O81" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.2">
@@ -26435,7 +26455,7 @@
       <c r="J82" s="49"/>
       <c r="K82" s="49"/>
       <c r="O82" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.2">
@@ -26465,7 +26485,7 @@
       <c r="J83" s="49"/>
       <c r="K83" s="49"/>
       <c r="O83" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.2">
@@ -26495,7 +26515,7 @@
       <c r="J84" s="49"/>
       <c r="K84" s="49"/>
       <c r="O84" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.2">
@@ -26537,7 +26557,9 @@
       <c r="N85">
         <v>100</v>
       </c>
-      <c r="O85" s="49"/>
+      <c r="O85" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86">
@@ -26566,7 +26588,7 @@
       <c r="J86" s="49"/>
       <c r="K86" s="49"/>
       <c r="O86" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.2">
@@ -26596,7 +26618,7 @@
       <c r="J87" s="49"/>
       <c r="K87" s="49"/>
       <c r="O87" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.2">
@@ -26626,7 +26648,7 @@
       <c r="J88" s="49"/>
       <c r="K88" s="49"/>
       <c r="O88" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.2">
@@ -26656,7 +26678,7 @@
       <c r="J89" s="49"/>
       <c r="K89" s="49"/>
       <c r="O89" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
@@ -26686,7 +26708,7 @@
       <c r="J90" s="49"/>
       <c r="K90" s="49"/>
       <c r="O90" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.2">
@@ -26716,7 +26738,7 @@
       <c r="J91" s="49"/>
       <c r="K91" s="49"/>
       <c r="O91" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
@@ -26758,7 +26780,9 @@
       <c r="N92">
         <v>0</v>
       </c>
-      <c r="O92" s="49"/>
+      <c r="O92" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93">
@@ -26779,7 +26803,7 @@
         <v>130776</v>
       </c>
       <c r="H93" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I93" s="51">
         <v>35</v>
@@ -26799,7 +26823,9 @@
       <c r="N93">
         <v>0</v>
       </c>
-      <c r="O93" s="49"/>
+      <c r="O93" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94">
@@ -26828,7 +26854,7 @@
       <c r="J94" s="49"/>
       <c r="K94" s="49"/>
       <c r="O94" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
@@ -26842,7 +26868,7 @@
         <v>183</v>
       </c>
       <c r="D95" s="48" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E95" s="48"/>
       <c r="F95" s="48"/>
@@ -26858,7 +26884,7 @@
       <c r="J95" s="49"/>
       <c r="K95" s="49"/>
       <c r="O95" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
@@ -26888,7 +26914,7 @@
       <c r="J96" s="49"/>
       <c r="K96" s="49"/>
       <c r="O96" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.2">
@@ -26930,7 +26956,9 @@
       <c r="N97">
         <v>0</v>
       </c>
-      <c r="O97" s="49"/>
+      <c r="O97" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98">
@@ -26959,7 +26987,7 @@
       <c r="J98" s="49"/>
       <c r="K98" s="49"/>
       <c r="O98" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.2">
@@ -26989,7 +27017,7 @@
       <c r="J99" s="49"/>
       <c r="K99" s="49"/>
       <c r="O99" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.2">
@@ -27031,7 +27059,9 @@
       <c r="N100">
         <v>100</v>
       </c>
-      <c r="O100" s="49"/>
+      <c r="O100" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101">
@@ -27060,7 +27090,7 @@
       <c r="J101" s="49"/>
       <c r="K101" s="49"/>
       <c r="O101" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.2">
@@ -27102,7 +27132,9 @@
       <c r="N102">
         <v>100</v>
       </c>
-      <c r="O102" s="49"/>
+      <c r="O102" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103">
@@ -27131,7 +27163,7 @@
       <c r="J103" s="49"/>
       <c r="K103" s="49"/>
       <c r="O103" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.2">
@@ -27173,7 +27205,9 @@
       <c r="N104">
         <v>100</v>
       </c>
-      <c r="O104" s="49"/>
+      <c r="O104" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105">
@@ -27214,7 +27248,9 @@
       <c r="N105">
         <v>100</v>
       </c>
-      <c r="O105" s="49"/>
+      <c r="O105" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106">
@@ -27243,7 +27279,7 @@
       <c r="J106" s="49"/>
       <c r="K106" s="49"/>
       <c r="O106" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.2">
@@ -27273,7 +27309,7 @@
       <c r="J107" s="49"/>
       <c r="K107" s="49"/>
       <c r="O107" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.2">
@@ -27303,7 +27339,7 @@
       <c r="J108" s="49"/>
       <c r="K108" s="49"/>
       <c r="O108" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.2">
@@ -27317,7 +27353,7 @@
         <v>183</v>
       </c>
       <c r="D109" s="48" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="E109" s="48"/>
       <c r="F109" s="48"/>
@@ -27333,7 +27369,7 @@
       <c r="J109" s="49"/>
       <c r="K109" s="49"/>
       <c r="O109" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.2">
@@ -27363,7 +27399,7 @@
       <c r="J110" s="49"/>
       <c r="K110" s="49"/>
       <c r="O110" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.2">
@@ -27393,7 +27429,7 @@
       <c r="J111" s="49"/>
       <c r="K111" s="49"/>
       <c r="O111" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.2">
@@ -27423,7 +27459,7 @@
       <c r="J112" s="49"/>
       <c r="K112" s="49"/>
       <c r="O112" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.2">
@@ -27453,7 +27489,7 @@
       <c r="J113" s="49"/>
       <c r="K113" s="49"/>
       <c r="O113" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.2">
@@ -27483,7 +27519,7 @@
       <c r="J114" s="49"/>
       <c r="K114" s="49"/>
       <c r="O114" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.2">
@@ -27513,7 +27549,7 @@
       <c r="J115" s="49"/>
       <c r="K115" s="49"/>
       <c r="O115" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.2">
@@ -27543,7 +27579,7 @@
       <c r="J116" s="49"/>
       <c r="K116" s="49"/>
       <c r="O116" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.2">
@@ -27585,7 +27621,9 @@
       <c r="N117">
         <v>0</v>
       </c>
-      <c r="O117" s="49"/>
+      <c r="O117" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118">
@@ -27614,7 +27652,7 @@
       <c r="J118" s="49"/>
       <c r="K118" s="49"/>
       <c r="O118" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.2">
@@ -27644,7 +27682,7 @@
       <c r="J119" s="49"/>
       <c r="K119" s="49"/>
       <c r="O119" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.2">
@@ -27674,7 +27712,7 @@
       <c r="J120" s="49"/>
       <c r="K120" s="49"/>
       <c r="O120" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.2">
@@ -27704,7 +27742,7 @@
       <c r="J121" s="49"/>
       <c r="K121" s="49"/>
       <c r="O121" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.2">
@@ -27734,7 +27772,7 @@
       <c r="J122" s="49"/>
       <c r="K122" s="49"/>
       <c r="O122" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.2">
@@ -27764,7 +27802,7 @@
       <c r="J123" s="49"/>
       <c r="K123" s="49"/>
       <c r="O123" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.2">
@@ -27794,7 +27832,7 @@
       <c r="J124" s="49"/>
       <c r="K124" s="49"/>
       <c r="O124" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.2">
@@ -27824,7 +27862,7 @@
       <c r="J125" s="49"/>
       <c r="K125" s="49"/>
       <c r="O125" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.2">
@@ -27854,7 +27892,7 @@
       <c r="J126" s="49"/>
       <c r="K126" s="49"/>
       <c r="O126" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.2">
@@ -27868,7 +27906,7 @@
         <v>213</v>
       </c>
       <c r="D127" s="48" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E127" s="48"/>
       <c r="F127" s="48"/>
@@ -27884,7 +27922,7 @@
       <c r="J127" s="49"/>
       <c r="K127" s="49"/>
       <c r="O127" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.2">
@@ -27914,7 +27952,7 @@
       <c r="J128" s="49"/>
       <c r="K128" s="49"/>
       <c r="O128" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.2">
@@ -27928,7 +27966,7 @@
         <v>213</v>
       </c>
       <c r="D129" s="48" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E129" s="48"/>
       <c r="F129" s="48"/>
@@ -27944,7 +27982,7 @@
       <c r="J129" s="49"/>
       <c r="K129" s="49"/>
       <c r="O129" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.2">
@@ -27974,7 +28012,7 @@
       <c r="J130" s="49"/>
       <c r="K130" s="49"/>
       <c r="O130" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.2">
@@ -28004,7 +28042,7 @@
       <c r="J131" s="49"/>
       <c r="K131" s="49"/>
       <c r="O131" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.2">
@@ -28034,7 +28072,7 @@
       <c r="J132" s="49"/>
       <c r="K132" s="49"/>
       <c r="O132" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.2">
@@ -28064,7 +28102,7 @@
       <c r="J133" s="49"/>
       <c r="K133" s="49"/>
       <c r="O133" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.2">
@@ -28106,7 +28144,9 @@
       <c r="N134">
         <v>67</v>
       </c>
-      <c r="O134" s="49"/>
+      <c r="O134" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A135">
@@ -28135,7 +28175,7 @@
       <c r="J135" s="49"/>
       <c r="K135" s="49"/>
       <c r="O135" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.2">
@@ -28165,7 +28205,7 @@
       <c r="J136" s="49"/>
       <c r="K136" s="49"/>
       <c r="O136" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.2">
@@ -28207,7 +28247,9 @@
       <c r="N137">
         <v>100</v>
       </c>
-      <c r="O137" s="49"/>
+      <c r="O137" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A138">
@@ -28236,7 +28278,7 @@
       <c r="J138" s="49"/>
       <c r="K138" s="49"/>
       <c r="O138" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.2">
@@ -28266,7 +28308,7 @@
       <c r="J139" s="49"/>
       <c r="K139" s="49"/>
       <c r="O139" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140" spans="1:15" x14ac:dyDescent="0.2">
@@ -28296,7 +28338,7 @@
       <c r="J140" s="49"/>
       <c r="K140" s="49"/>
       <c r="O140" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.2">
@@ -28326,7 +28368,7 @@
       <c r="J141" s="49"/>
       <c r="K141" s="49"/>
       <c r="O141" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.2">
@@ -28368,7 +28410,9 @@
       <c r="N142">
         <v>100</v>
       </c>
-      <c r="O142" s="49"/>
+      <c r="O142" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A143">
@@ -28397,7 +28441,7 @@
       <c r="J143" s="49"/>
       <c r="K143" s="49"/>
       <c r="O143" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144" spans="1:15" x14ac:dyDescent="0.2">
@@ -28427,7 +28471,7 @@
       <c r="J144" s="49"/>
       <c r="K144" s="49"/>
       <c r="O144" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="145" spans="1:15" x14ac:dyDescent="0.2">
@@ -28457,7 +28501,7 @@
       <c r="J145" s="49"/>
       <c r="K145" s="49"/>
       <c r="O145" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="146" spans="1:15" x14ac:dyDescent="0.2">
@@ -28487,7 +28531,7 @@
       <c r="J146" s="49"/>
       <c r="K146" s="49"/>
       <c r="O146" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="147" spans="1:15" x14ac:dyDescent="0.2">
@@ -28529,7 +28573,9 @@
       <c r="N147">
         <v>100</v>
       </c>
-      <c r="O147" s="49"/>
+      <c r="O147" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="148" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A148">
@@ -28558,7 +28604,7 @@
       <c r="J148" s="49"/>
       <c r="K148" s="49"/>
       <c r="O148" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="149" spans="1:15" x14ac:dyDescent="0.2">
@@ -28588,7 +28634,7 @@
       <c r="J149" s="49"/>
       <c r="K149" s="49"/>
       <c r="O149" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="150" spans="1:15" x14ac:dyDescent="0.2">
@@ -28618,7 +28664,7 @@
       <c r="J150" s="49"/>
       <c r="K150" s="49"/>
       <c r="O150" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="151" spans="1:15" x14ac:dyDescent="0.2">
@@ -28648,7 +28694,7 @@
       <c r="J151" s="49"/>
       <c r="K151" s="49"/>
       <c r="O151" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="152" spans="1:15" x14ac:dyDescent="0.2">
@@ -28690,7 +28736,9 @@
       <c r="N152">
         <v>100</v>
       </c>
-      <c r="O152" s="49"/>
+      <c r="O152" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="153" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A153">
@@ -28719,7 +28767,7 @@
       <c r="J153" s="49"/>
       <c r="K153" s="49"/>
       <c r="O153" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="154" spans="1:15" x14ac:dyDescent="0.2">
@@ -28761,7 +28809,9 @@
       <c r="N154">
         <v>100</v>
       </c>
-      <c r="O154" s="49"/>
+      <c r="O154" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="155" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A155">
@@ -28790,7 +28840,7 @@
       <c r="J155" s="49"/>
       <c r="K155" s="49"/>
       <c r="O155" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="156" spans="1:15" x14ac:dyDescent="0.2">
@@ -28820,7 +28870,7 @@
       <c r="J156" s="49"/>
       <c r="K156" s="49"/>
       <c r="O156" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="157" spans="1:15" x14ac:dyDescent="0.2">
@@ -28850,7 +28900,7 @@
       <c r="J157" s="49"/>
       <c r="K157" s="49"/>
       <c r="O157" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.2">
@@ -28880,7 +28930,7 @@
       <c r="J158" s="49"/>
       <c r="K158" s="49"/>
       <c r="O158" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="159" spans="1:15" x14ac:dyDescent="0.2">
@@ -28922,7 +28972,9 @@
       <c r="N159">
         <v>100</v>
       </c>
-      <c r="O159" s="49"/>
+      <c r="O159" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="160" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A160">
@@ -28963,7 +29015,9 @@
       <c r="N160">
         <v>0</v>
       </c>
-      <c r="O160" s="49"/>
+      <c r="O160" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="161" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A161">
@@ -29004,7 +29058,9 @@
       <c r="N161">
         <v>0</v>
       </c>
-      <c r="O161" s="49"/>
+      <c r="O161" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="162" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A162">
@@ -29033,7 +29089,7 @@
       <c r="J162" s="49"/>
       <c r="K162" s="49"/>
       <c r="O162" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="163" spans="1:15" x14ac:dyDescent="0.2">
@@ -29075,7 +29131,9 @@
       <c r="N163">
         <v>0</v>
       </c>
-      <c r="O163" s="49"/>
+      <c r="O163" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="164" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A164">
@@ -29104,7 +29162,7 @@
       <c r="J164" s="49"/>
       <c r="K164" s="49"/>
       <c r="O164" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="165" spans="1:15" x14ac:dyDescent="0.2">
@@ -29134,7 +29192,7 @@
       <c r="J165" s="49"/>
       <c r="K165" s="49"/>
       <c r="O165" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="166" spans="1:15" x14ac:dyDescent="0.2">
@@ -29176,7 +29234,9 @@
       <c r="N166">
         <v>0</v>
       </c>
-      <c r="O166" s="49"/>
+      <c r="O166" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A167">
@@ -29217,7 +29277,9 @@
       <c r="N167">
         <v>0</v>
       </c>
-      <c r="O167" s="49"/>
+      <c r="O167" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="168" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A168">
@@ -29246,7 +29308,7 @@
       <c r="J168" s="49"/>
       <c r="K168" s="49"/>
       <c r="O168" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="169" spans="1:15" x14ac:dyDescent="0.2">
@@ -29276,7 +29338,7 @@
       <c r="J169" s="49"/>
       <c r="K169" s="49"/>
       <c r="O169" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="170" spans="1:15" x14ac:dyDescent="0.2">
@@ -29306,7 +29368,7 @@
       <c r="J170" s="49"/>
       <c r="K170" s="49"/>
       <c r="O170" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="171" spans="1:15" x14ac:dyDescent="0.2">
@@ -29336,7 +29398,7 @@
       <c r="J171" s="49"/>
       <c r="K171" s="49"/>
       <c r="O171" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="172" spans="1:15" x14ac:dyDescent="0.2">
@@ -29366,7 +29428,7 @@
       <c r="J172" s="49"/>
       <c r="K172" s="49"/>
       <c r="O172" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="173" spans="1:15" x14ac:dyDescent="0.2">
@@ -29396,7 +29458,7 @@
       <c r="J173" s="49"/>
       <c r="K173" s="49"/>
       <c r="O173" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="174" spans="1:15" x14ac:dyDescent="0.2">
@@ -29426,7 +29488,7 @@
       <c r="J174" s="49"/>
       <c r="K174" s="49"/>
       <c r="O174" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="175" spans="1:15" x14ac:dyDescent="0.2">
@@ -29456,7 +29518,7 @@
       <c r="J175" s="49"/>
       <c r="K175" s="49"/>
       <c r="O175" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="176" spans="1:15" x14ac:dyDescent="0.2">
@@ -29486,7 +29548,7 @@
       <c r="J176" s="49"/>
       <c r="K176" s="49"/>
       <c r="O176" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.2">
@@ -29516,7 +29578,7 @@
       <c r="J177" s="49"/>
       <c r="K177" s="49"/>
       <c r="O177" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="178" spans="1:15" x14ac:dyDescent="0.2">
@@ -29558,7 +29620,9 @@
       <c r="N178">
         <v>100</v>
       </c>
-      <c r="O178" s="49"/>
+      <c r="O178" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="179" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A179">
@@ -29571,7 +29635,7 @@
         <v>258</v>
       </c>
       <c r="D179" s="48" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="E179" s="48"/>
       <c r="F179" s="48"/>
@@ -29587,7 +29651,7 @@
       <c r="J179" s="49"/>
       <c r="K179" s="49"/>
       <c r="O179" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.2">
@@ -29617,7 +29681,7 @@
       <c r="J180" s="49"/>
       <c r="K180" s="49"/>
       <c r="O180" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="181" spans="1:15" x14ac:dyDescent="0.2">
@@ -29659,7 +29723,9 @@
       <c r="N181">
         <v>100</v>
       </c>
-      <c r="O181" s="49"/>
+      <c r="O181" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="182" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A182">
@@ -29688,7 +29754,7 @@
       <c r="J182" s="49"/>
       <c r="K182" s="49"/>
       <c r="O182" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="183" spans="1:15" x14ac:dyDescent="0.2">
@@ -29718,7 +29784,7 @@
       <c r="J183" s="49"/>
       <c r="K183" s="49"/>
       <c r="O183" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="184" spans="1:15" x14ac:dyDescent="0.2">
@@ -29748,7 +29814,7 @@
       <c r="J184" s="49"/>
       <c r="K184" s="49"/>
       <c r="O184" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="185" spans="1:15" x14ac:dyDescent="0.2">
@@ -29778,7 +29844,7 @@
       <c r="J185" s="49"/>
       <c r="K185" s="49"/>
       <c r="O185" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="186" spans="1:15" x14ac:dyDescent="0.2">
@@ -29792,7 +29858,7 @@
         <v>258</v>
       </c>
       <c r="D186" s="48" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="E186" s="48"/>
       <c r="F186" s="48"/>
@@ -29808,7 +29874,7 @@
       <c r="J186" s="49"/>
       <c r="K186" s="49"/>
       <c r="O186" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="187" spans="1:15" x14ac:dyDescent="0.2">
@@ -29838,7 +29904,7 @@
       <c r="J187" s="49"/>
       <c r="K187" s="49"/>
       <c r="O187" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="188" spans="1:15" x14ac:dyDescent="0.2">
@@ -29868,7 +29934,7 @@
       <c r="J188" s="49"/>
       <c r="K188" s="49"/>
       <c r="O188" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="189" spans="1:15" x14ac:dyDescent="0.2">
@@ -29898,7 +29964,7 @@
       <c r="J189" s="49"/>
       <c r="K189" s="49"/>
       <c r="O189" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="190" spans="1:15" x14ac:dyDescent="0.2">
@@ -29940,7 +30006,9 @@
       <c r="N190">
         <v>0</v>
       </c>
-      <c r="O190" s="49"/>
+      <c r="O190" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="191" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A191">
@@ -29969,7 +30037,7 @@
       <c r="J191" s="49"/>
       <c r="K191" s="49"/>
       <c r="O191" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="192" spans="1:15" x14ac:dyDescent="0.2">
@@ -29999,7 +30067,7 @@
       <c r="J192" s="49"/>
       <c r="K192" s="49"/>
       <c r="O192" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="193" spans="1:15" x14ac:dyDescent="0.2">
@@ -30029,7 +30097,7 @@
       <c r="J193" s="49"/>
       <c r="K193" s="49"/>
       <c r="O193" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="194" spans="1:15" x14ac:dyDescent="0.2">
@@ -30059,7 +30127,7 @@
       <c r="J194" s="49"/>
       <c r="K194" s="49"/>
       <c r="O194" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="195" spans="1:15" x14ac:dyDescent="0.2">
@@ -30089,7 +30157,7 @@
       <c r="J195" s="49"/>
       <c r="K195" s="49"/>
       <c r="O195" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="196" spans="1:15" x14ac:dyDescent="0.2">
@@ -30119,7 +30187,7 @@
       <c r="J196" s="49"/>
       <c r="K196" s="49"/>
       <c r="O196" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="197" spans="1:15" x14ac:dyDescent="0.2">
@@ -30149,7 +30217,7 @@
       <c r="J197" s="49"/>
       <c r="K197" s="49"/>
       <c r="O197" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="198" spans="1:15" x14ac:dyDescent="0.2">
@@ -30179,7 +30247,7 @@
       <c r="J198" s="49"/>
       <c r="K198" s="49"/>
       <c r="O198" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="199" spans="1:15" x14ac:dyDescent="0.2">
@@ -30209,7 +30277,7 @@
       <c r="J199" s="49"/>
       <c r="K199" s="49"/>
       <c r="O199" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="200" spans="1:15" x14ac:dyDescent="0.2">
@@ -30239,7 +30307,7 @@
       <c r="J200" s="49"/>
       <c r="K200" s="49"/>
       <c r="O200" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="201" spans="1:15" x14ac:dyDescent="0.2">
@@ -30253,7 +30321,7 @@
         <v>213</v>
       </c>
       <c r="D201" s="48" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="E201" s="48"/>
       <c r="F201" s="48"/>
@@ -30281,7 +30349,9 @@
       <c r="N201">
         <v>0</v>
       </c>
-      <c r="O201" s="49"/>
+      <c r="O201" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="202" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A202">
@@ -30310,7 +30380,7 @@
       <c r="J202" s="49"/>
       <c r="K202" s="49"/>
       <c r="O202" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="203" spans="1:15" x14ac:dyDescent="0.2">
@@ -30340,7 +30410,7 @@
       <c r="J203" s="49"/>
       <c r="K203" s="49"/>
       <c r="O203" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="204" spans="1:15" x14ac:dyDescent="0.2">
@@ -30370,7 +30440,7 @@
       <c r="J204" s="49"/>
       <c r="K204" s="49"/>
       <c r="O204" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="205" spans="1:15" x14ac:dyDescent="0.2">
@@ -30400,7 +30470,7 @@
       <c r="J205" s="49"/>
       <c r="K205" s="49"/>
       <c r="O205" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="206" spans="1:15" x14ac:dyDescent="0.2">
@@ -30430,7 +30500,7 @@
       <c r="J206" s="49"/>
       <c r="K206" s="49"/>
       <c r="O206" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="207" spans="1:15" x14ac:dyDescent="0.2">
@@ -30472,7 +30542,9 @@
       <c r="N207">
         <v>0</v>
       </c>
-      <c r="O207" s="49"/>
+      <c r="O207" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="208" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A208">
@@ -30501,7 +30573,7 @@
       <c r="J208" s="49"/>
       <c r="K208" s="49"/>
       <c r="O208" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="209" spans="1:15" x14ac:dyDescent="0.2">
@@ -30531,7 +30603,7 @@
       <c r="J209" s="49"/>
       <c r="K209" s="49"/>
       <c r="O209" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="210" spans="1:15" x14ac:dyDescent="0.2">
@@ -30561,7 +30633,7 @@
       <c r="J210" s="49"/>
       <c r="K210" s="49"/>
       <c r="O210" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="211" spans="1:15" x14ac:dyDescent="0.2">
@@ -30591,7 +30663,7 @@
       <c r="J211" s="49"/>
       <c r="K211" s="49"/>
       <c r="O211" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="212" spans="1:15" x14ac:dyDescent="0.2">
@@ -30621,7 +30693,7 @@
       <c r="J212" s="49"/>
       <c r="K212" s="49"/>
       <c r="O212" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="213" spans="1:15" x14ac:dyDescent="0.2">
@@ -30663,7 +30735,9 @@
       <c r="N213">
         <v>0</v>
       </c>
-      <c r="O213" s="49"/>
+      <c r="O213" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="214" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A214">
@@ -30692,7 +30766,7 @@
       <c r="J214" s="49"/>
       <c r="K214" s="49"/>
       <c r="O214" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="215" spans="1:15" x14ac:dyDescent="0.2">
@@ -30734,7 +30808,9 @@
       <c r="N215">
         <v>0</v>
       </c>
-      <c r="O215" s="49"/>
+      <c r="O215" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="216" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A216">
@@ -30763,7 +30839,7 @@
       <c r="J216" s="49"/>
       <c r="K216" s="49"/>
       <c r="O216" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="217" spans="1:15" x14ac:dyDescent="0.2">
@@ -30793,7 +30869,7 @@
       <c r="J217" s="49"/>
       <c r="K217" s="49"/>
       <c r="O217" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="218" spans="1:15" x14ac:dyDescent="0.2">
@@ -30835,7 +30911,9 @@
       <c r="N218">
         <v>0</v>
       </c>
-      <c r="O218" s="49"/>
+      <c r="O218" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="219" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A219">
@@ -30864,7 +30942,7 @@
       <c r="J219" s="49"/>
       <c r="K219" s="49"/>
       <c r="O219" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="220" spans="1:15" x14ac:dyDescent="0.2">
@@ -30878,7 +30956,7 @@
         <v>296</v>
       </c>
       <c r="D220" s="48" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="E220" s="48"/>
       <c r="F220" s="48"/>
@@ -30894,7 +30972,7 @@
       <c r="J220" s="49"/>
       <c r="K220" s="49"/>
       <c r="O220" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="221" spans="1:15" x14ac:dyDescent="0.2">
@@ -30924,7 +31002,7 @@
       <c r="J221" s="49"/>
       <c r="K221" s="49"/>
       <c r="O221" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="222" spans="1:15" x14ac:dyDescent="0.2">
@@ -30954,7 +31032,7 @@
       <c r="J222" s="49"/>
       <c r="K222" s="49"/>
       <c r="O222" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="223" spans="1:15" x14ac:dyDescent="0.2">
@@ -30984,7 +31062,7 @@
       <c r="J223" s="49"/>
       <c r="K223" s="49"/>
       <c r="O223" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="224" spans="1:15" x14ac:dyDescent="0.2">
@@ -30998,7 +31076,7 @@
         <v>304</v>
       </c>
       <c r="D224" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="E224" s="48"/>
       <c r="F224" s="48"/>
@@ -31026,7 +31104,9 @@
       <c r="N224">
         <v>0</v>
       </c>
-      <c r="O224" s="49"/>
+      <c r="O224" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="225" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A225">
@@ -31055,7 +31135,7 @@
       <c r="J225" s="49"/>
       <c r="K225" s="49"/>
       <c r="O225" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="226" spans="1:15" x14ac:dyDescent="0.2">
@@ -31085,7 +31165,7 @@
       <c r="J226" s="49"/>
       <c r="K226" s="49"/>
       <c r="O226" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="227" spans="1:15" x14ac:dyDescent="0.2">
@@ -31115,7 +31195,7 @@
       <c r="J227" s="49"/>
       <c r="K227" s="49"/>
       <c r="O227" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="228" spans="1:15" x14ac:dyDescent="0.2">
@@ -31145,7 +31225,7 @@
       <c r="J228" s="49"/>
       <c r="K228" s="49"/>
       <c r="O228" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="229" spans="1:15" x14ac:dyDescent="0.2">
@@ -31175,7 +31255,7 @@
       <c r="J229" s="49"/>
       <c r="K229" s="49"/>
       <c r="O229" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="230" spans="1:15" x14ac:dyDescent="0.2">
@@ -31205,7 +31285,7 @@
       <c r="J230" s="49"/>
       <c r="K230" s="49"/>
       <c r="O230" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="231" spans="1:15" x14ac:dyDescent="0.2">
@@ -31235,7 +31315,7 @@
       <c r="J231" s="49"/>
       <c r="K231" s="49"/>
       <c r="O231" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="232" spans="1:15" x14ac:dyDescent="0.2">
@@ -31265,7 +31345,7 @@
       <c r="J232" s="49"/>
       <c r="K232" s="49"/>
       <c r="O232" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="233" spans="1:15" x14ac:dyDescent="0.2">
@@ -31295,7 +31375,7 @@
       <c r="J233" s="49"/>
       <c r="K233" s="49"/>
       <c r="O233" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="234" spans="1:15" x14ac:dyDescent="0.2">
@@ -31325,7 +31405,7 @@
       <c r="J234" s="49"/>
       <c r="K234" s="49"/>
       <c r="O234" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="235" spans="1:15" x14ac:dyDescent="0.2">
@@ -31355,7 +31435,7 @@
       <c r="J235" s="49"/>
       <c r="K235" s="49"/>
       <c r="O235" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="236" spans="1:15" x14ac:dyDescent="0.2">
@@ -31385,7 +31465,7 @@
       <c r="J236" s="49"/>
       <c r="K236" s="49"/>
       <c r="O236" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="237" spans="1:15" x14ac:dyDescent="0.2">
@@ -31415,7 +31495,7 @@
       <c r="J237" s="49"/>
       <c r="K237" s="49"/>
       <c r="O237" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="238" spans="1:15" x14ac:dyDescent="0.2">
@@ -31445,7 +31525,7 @@
       <c r="J238" s="49"/>
       <c r="K238" s="49"/>
       <c r="O238" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="239" spans="1:15" x14ac:dyDescent="0.2">
@@ -31475,7 +31555,7 @@
       <c r="J239" s="49"/>
       <c r="K239" s="49"/>
       <c r="O239" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="240" spans="1:15" x14ac:dyDescent="0.2">
@@ -31505,7 +31585,7 @@
       <c r="J240" s="49"/>
       <c r="K240" s="49"/>
       <c r="O240" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="241" spans="1:15" x14ac:dyDescent="0.2">
@@ -31535,7 +31615,7 @@
       <c r="J241" s="49"/>
       <c r="K241" s="49"/>
       <c r="O241" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="242" spans="1:15" x14ac:dyDescent="0.2">
@@ -31577,7 +31657,9 @@
       <c r="N242">
         <v>0</v>
       </c>
-      <c r="O242" s="49"/>
+      <c r="O242" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="243" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A243">
@@ -31606,7 +31688,7 @@
       <c r="J243" s="49"/>
       <c r="K243" s="49"/>
       <c r="O243" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="244" spans="1:15" x14ac:dyDescent="0.2">
@@ -31636,7 +31718,7 @@
       <c r="J244" s="49"/>
       <c r="K244" s="49"/>
       <c r="O244" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="245" spans="1:15" x14ac:dyDescent="0.2">
@@ -31650,7 +31732,7 @@
         <v>320</v>
       </c>
       <c r="D245" s="48" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="E245" s="48"/>
       <c r="F245" s="48"/>
@@ -31666,7 +31748,7 @@
       <c r="J245" s="49"/>
       <c r="K245" s="49"/>
       <c r="O245" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="246" spans="1:15" x14ac:dyDescent="0.2">
@@ -31696,7 +31778,7 @@
       <c r="J246" s="49"/>
       <c r="K246" s="49"/>
       <c r="O246" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="247" spans="1:15" x14ac:dyDescent="0.2">
@@ -31738,7 +31820,9 @@
       <c r="N247">
         <v>100</v>
       </c>
-      <c r="O247" s="49"/>
+      <c r="O247" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="248" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A248">
@@ -31767,7 +31851,7 @@
       <c r="J248" s="49"/>
       <c r="K248" s="49"/>
       <c r="O248" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="249" spans="1:15" x14ac:dyDescent="0.2">
@@ -31797,7 +31881,7 @@
       <c r="J249" s="49"/>
       <c r="K249" s="49"/>
       <c r="O249" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="250" spans="1:15" x14ac:dyDescent="0.2">
@@ -31827,7 +31911,7 @@
       <c r="J250" s="49"/>
       <c r="K250" s="49"/>
       <c r="O250" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="251" spans="1:15" x14ac:dyDescent="0.2">
@@ -31857,7 +31941,7 @@
       <c r="J251" s="49"/>
       <c r="K251" s="49"/>
       <c r="O251" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="252" spans="1:15" x14ac:dyDescent="0.2">
@@ -31887,7 +31971,7 @@
       <c r="J252" s="49"/>
       <c r="K252" s="49"/>
       <c r="O252" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="253" spans="1:15" x14ac:dyDescent="0.2">
@@ -31917,7 +32001,7 @@
       <c r="J253" s="49"/>
       <c r="K253" s="49"/>
       <c r="O253" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="254" spans="1:15" x14ac:dyDescent="0.2">
@@ -31947,7 +32031,7 @@
       <c r="J254" s="49"/>
       <c r="K254" s="49"/>
       <c r="O254" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="255" spans="1:15" x14ac:dyDescent="0.2">
@@ -31977,7 +32061,7 @@
       <c r="J255" s="49"/>
       <c r="K255" s="49"/>
       <c r="O255" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="256" spans="1:15" x14ac:dyDescent="0.2">
@@ -32007,7 +32091,7 @@
       <c r="J256" s="49"/>
       <c r="K256" s="49"/>
       <c r="O256" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="257" spans="1:15" x14ac:dyDescent="0.2">
@@ -32037,7 +32121,7 @@
       <c r="J257" s="49"/>
       <c r="K257" s="49"/>
       <c r="O257" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="258" spans="1:15" x14ac:dyDescent="0.2">
@@ -32067,7 +32151,7 @@
       <c r="J258" s="49"/>
       <c r="K258" s="49"/>
       <c r="O258" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="259" spans="1:15" x14ac:dyDescent="0.2">
@@ -32097,7 +32181,7 @@
       <c r="J259" s="49"/>
       <c r="K259" s="49"/>
       <c r="O259" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="260" spans="1:15" x14ac:dyDescent="0.2">
@@ -32127,7 +32211,7 @@
       <c r="J260" s="49"/>
       <c r="K260" s="49"/>
       <c r="O260" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="261" spans="1:15" x14ac:dyDescent="0.2">
@@ -32157,7 +32241,7 @@
       <c r="J261" s="49"/>
       <c r="K261" s="49"/>
       <c r="O261" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="262" spans="1:15" x14ac:dyDescent="0.2">
@@ -32187,7 +32271,7 @@
       <c r="J262" s="49"/>
       <c r="K262" s="49"/>
       <c r="O262" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="263" spans="1:15" x14ac:dyDescent="0.2">
@@ -32229,7 +32313,9 @@
       <c r="N263">
         <v>0</v>
       </c>
-      <c r="O263" s="49"/>
+      <c r="O263" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="264" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A264">
@@ -32258,7 +32344,7 @@
       <c r="J264" s="49"/>
       <c r="K264" s="49"/>
       <c r="O264" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="265" spans="1:15" x14ac:dyDescent="0.2">
@@ -32300,7 +32386,9 @@
       <c r="N265">
         <v>0</v>
       </c>
-      <c r="O265" s="49"/>
+      <c r="O265" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="266" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A266">
@@ -32329,7 +32417,7 @@
       <c r="J266" s="49"/>
       <c r="K266" s="49"/>
       <c r="O266" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="267" spans="1:15" x14ac:dyDescent="0.2">
@@ -32359,7 +32447,7 @@
       <c r="J267" s="49"/>
       <c r="K267" s="49"/>
       <c r="O267" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="268" spans="1:15" x14ac:dyDescent="0.2">
@@ -32389,7 +32477,7 @@
       <c r="J268" s="49"/>
       <c r="K268" s="49"/>
       <c r="O268" s="49" t="s">
-        <v>423</v>
+        <v>92</v>
       </c>
     </row>
     <row r="269" spans="1:15" x14ac:dyDescent="0.2">
@@ -32431,7 +32519,9 @@
       <c r="N269">
         <v>0</v>
       </c>
-      <c r="O269" s="49"/>
+      <c r="O269" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="270" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A270">
@@ -32460,7 +32550,7 @@
       <c r="J270" s="49"/>
       <c r="K270" s="49"/>
       <c r="O270" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="271" spans="1:15" x14ac:dyDescent="0.2">
@@ -32490,7 +32580,7 @@
       <c r="J271" s="49"/>
       <c r="K271" s="49"/>
       <c r="O271" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="272" spans="1:15" x14ac:dyDescent="0.2">
@@ -32532,7 +32622,9 @@
       <c r="N272">
         <v>0</v>
       </c>
-      <c r="O272" s="49"/>
+      <c r="O272" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="273" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A273">
@@ -32561,7 +32653,7 @@
       <c r="J273" s="49"/>
       <c r="K273" s="49"/>
       <c r="O273" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="274" spans="1:15" x14ac:dyDescent="0.2">
@@ -32603,7 +32695,9 @@
       <c r="N274">
         <v>0</v>
       </c>
-      <c r="O274" s="49"/>
+      <c r="O274" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="275" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A275">
@@ -32644,7 +32738,9 @@
       <c r="N275">
         <v>100</v>
       </c>
-      <c r="O275" s="49"/>
+      <c r="O275" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="276" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A276">
@@ -32685,7 +32781,9 @@
       <c r="N276">
         <v>0</v>
       </c>
-      <c r="O276" s="49"/>
+      <c r="O276" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="277" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A277">
@@ -32714,7 +32812,7 @@
       <c r="J277" s="49"/>
       <c r="K277" s="49"/>
       <c r="O277" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="278" spans="1:15" x14ac:dyDescent="0.2">
@@ -32744,7 +32842,7 @@
       <c r="J278" s="49"/>
       <c r="K278" s="49"/>
       <c r="O278" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="279" spans="1:15" x14ac:dyDescent="0.2">
@@ -32774,7 +32872,7 @@
       <c r="J279" s="49"/>
       <c r="K279" s="49"/>
       <c r="O279" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="280" spans="1:15" x14ac:dyDescent="0.2">
@@ -32816,7 +32914,9 @@
       <c r="N280">
         <v>0</v>
       </c>
-      <c r="O280" s="49"/>
+      <c r="O280" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="281" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A281">
@@ -32845,7 +32945,7 @@
       <c r="J281" s="49"/>
       <c r="K281" s="49"/>
       <c r="O281" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="282" spans="1:15" x14ac:dyDescent="0.2">
@@ -32875,7 +32975,7 @@
       <c r="J282" s="49"/>
       <c r="K282" s="49"/>
       <c r="O282" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="283" spans="1:15" x14ac:dyDescent="0.2">
@@ -32905,7 +33005,7 @@
       <c r="J283" s="49"/>
       <c r="K283" s="49"/>
       <c r="O283" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="284" spans="1:15" x14ac:dyDescent="0.2">
@@ -32935,7 +33035,7 @@
       <c r="J284" s="49"/>
       <c r="K284" s="49"/>
       <c r="O284" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="285" spans="1:15" x14ac:dyDescent="0.2">
@@ -32965,7 +33065,7 @@
       <c r="J285" s="49"/>
       <c r="K285" s="49"/>
       <c r="O285" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="286" spans="1:15" x14ac:dyDescent="0.2">
@@ -32995,7 +33095,7 @@
       <c r="J286" s="49"/>
       <c r="K286" s="49"/>
       <c r="O286" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="287" spans="1:15" x14ac:dyDescent="0.2">
@@ -33025,7 +33125,7 @@
       <c r="J287" s="49"/>
       <c r="K287" s="49"/>
       <c r="O287" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="288" spans="1:15" x14ac:dyDescent="0.2">
@@ -33055,7 +33155,7 @@
       <c r="J288" s="49"/>
       <c r="K288" s="49"/>
       <c r="O288" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="289" spans="1:15" x14ac:dyDescent="0.2">
@@ -33085,7 +33185,7 @@
       <c r="J289" s="49"/>
       <c r="K289" s="49"/>
       <c r="O289" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="290" spans="1:15" x14ac:dyDescent="0.2">
@@ -33115,7 +33215,7 @@
       <c r="J290" s="49"/>
       <c r="K290" s="49"/>
       <c r="O290" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="291" spans="1:15" x14ac:dyDescent="0.2">
@@ -33145,7 +33245,7 @@
       <c r="J291" s="49"/>
       <c r="K291" s="49"/>
       <c r="O291" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="292" spans="1:15" x14ac:dyDescent="0.2">
@@ -33175,7 +33275,7 @@
       <c r="J292" s="49"/>
       <c r="K292" s="49"/>
       <c r="O292" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="293" spans="1:15" x14ac:dyDescent="0.2">
@@ -33205,7 +33305,7 @@
       <c r="J293" s="49"/>
       <c r="K293" s="49"/>
       <c r="O293" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="294" spans="1:15" x14ac:dyDescent="0.2">
@@ -33235,7 +33335,7 @@
       <c r="J294" s="49"/>
       <c r="K294" s="49"/>
       <c r="O294" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="295" spans="1:15" x14ac:dyDescent="0.2">
@@ -33265,7 +33365,7 @@
       <c r="J295" s="49"/>
       <c r="K295" s="49"/>
       <c r="O295" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="296" spans="1:15" x14ac:dyDescent="0.2">
@@ -33295,7 +33395,7 @@
       <c r="J296" s="49"/>
       <c r="K296" s="49"/>
       <c r="O296" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="297" spans="1:15" x14ac:dyDescent="0.2">
@@ -33325,7 +33425,7 @@
       <c r="J297" s="49"/>
       <c r="K297" s="49"/>
       <c r="O297" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="298" spans="1:15" x14ac:dyDescent="0.2">
@@ -33355,7 +33455,7 @@
       <c r="J298" s="49"/>
       <c r="K298" s="49"/>
       <c r="O298" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="299" spans="1:15" x14ac:dyDescent="0.2">
@@ -33385,7 +33485,7 @@
       <c r="J299" s="49"/>
       <c r="K299" s="49"/>
       <c r="O299" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="300" spans="1:15" x14ac:dyDescent="0.2">
@@ -33415,7 +33515,7 @@
       <c r="J300" s="49"/>
       <c r="K300" s="49"/>
       <c r="O300" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="301" spans="1:15" x14ac:dyDescent="0.2">
@@ -33445,7 +33545,7 @@
       <c r="J301" s="49"/>
       <c r="K301" s="49"/>
       <c r="O301" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="302" spans="1:15" x14ac:dyDescent="0.2">
@@ -33475,7 +33575,7 @@
       <c r="J302" s="49"/>
       <c r="K302" s="49"/>
       <c r="O302" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="303" spans="1:15" x14ac:dyDescent="0.2">
@@ -33505,7 +33605,7 @@
       <c r="J303" s="49"/>
       <c r="K303" s="49"/>
       <c r="O303" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="304" spans="1:15" x14ac:dyDescent="0.2">
@@ -33535,7 +33635,7 @@
       <c r="J304" s="49"/>
       <c r="K304" s="49"/>
       <c r="O304" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="305" spans="1:15" x14ac:dyDescent="0.2">
@@ -33565,7 +33665,7 @@
       <c r="J305" s="49"/>
       <c r="K305" s="49"/>
       <c r="O305" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="306" spans="1:15" x14ac:dyDescent="0.2">
@@ -33595,7 +33695,7 @@
       <c r="J306" s="49"/>
       <c r="K306" s="49"/>
       <c r="O306" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="307" spans="1:15" x14ac:dyDescent="0.2">
@@ -33625,7 +33725,7 @@
       <c r="J307" s="49"/>
       <c r="K307" s="49"/>
       <c r="O307" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="308" spans="1:15" x14ac:dyDescent="0.2">
@@ -33655,7 +33755,7 @@
       <c r="J308" s="49"/>
       <c r="K308" s="49"/>
       <c r="O308" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="309" spans="1:15" x14ac:dyDescent="0.2">
@@ -33697,7 +33797,9 @@
       <c r="N309">
         <v>100</v>
       </c>
-      <c r="O309" s="49"/>
+      <c r="O309" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="310" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A310">
@@ -33726,7 +33828,7 @@
       <c r="J310" s="49"/>
       <c r="K310" s="49"/>
       <c r="O310" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="311" spans="1:15" x14ac:dyDescent="0.2">
@@ -33756,7 +33858,7 @@
       <c r="J311" s="49"/>
       <c r="K311" s="49"/>
       <c r="O311" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="312" spans="1:15" x14ac:dyDescent="0.2">
@@ -33786,7 +33888,7 @@
       <c r="J312" s="49"/>
       <c r="K312" s="49"/>
       <c r="O312" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="313" spans="1:15" x14ac:dyDescent="0.2">
@@ -33816,7 +33918,7 @@
       <c r="J313" s="49"/>
       <c r="K313" s="49"/>
       <c r="O313" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="314" spans="1:15" x14ac:dyDescent="0.2">
@@ -33846,7 +33948,7 @@
       <c r="J314" s="49"/>
       <c r="K314" s="49"/>
       <c r="O314" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="315" spans="1:15" x14ac:dyDescent="0.2">
@@ -33876,7 +33978,7 @@
       <c r="J315" s="49"/>
       <c r="K315" s="49"/>
       <c r="O315" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="316" spans="1:15" x14ac:dyDescent="0.2">
@@ -33906,7 +34008,7 @@
       <c r="J316" s="49"/>
       <c r="K316" s="49"/>
       <c r="O316" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="317" spans="1:15" x14ac:dyDescent="0.2">
@@ -33936,7 +34038,7 @@
       <c r="J317" s="49"/>
       <c r="K317" s="49"/>
       <c r="O317" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="318" spans="1:15" x14ac:dyDescent="0.2">
@@ -33966,7 +34068,7 @@
       <c r="J318" s="49"/>
       <c r="K318" s="49"/>
       <c r="O318" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="319" spans="1:15" x14ac:dyDescent="0.2">
@@ -33996,7 +34098,7 @@
       <c r="J319" s="49"/>
       <c r="K319" s="49"/>
       <c r="O319" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="320" spans="1:15" x14ac:dyDescent="0.2">
@@ -34026,7 +34128,7 @@
       <c r="J320" s="49"/>
       <c r="K320" s="49"/>
       <c r="O320" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="321" spans="1:15" x14ac:dyDescent="0.2">
@@ -34068,7 +34170,9 @@
       <c r="N321">
         <v>100</v>
       </c>
-      <c r="O321" s="49"/>
+      <c r="O321" s="49" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="322" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A322">
@@ -34097,7 +34201,7 @@
       <c r="J322" s="49"/>
       <c r="K322" s="49"/>
       <c r="O322" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="323" spans="1:15" x14ac:dyDescent="0.2">
@@ -34127,7 +34231,7 @@
       <c r="J323" s="49"/>
       <c r="K323" s="49"/>
       <c r="O323" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="324" spans="1:15" x14ac:dyDescent="0.2">
@@ -34157,7 +34261,7 @@
       <c r="J324" s="49"/>
       <c r="K324" s="49"/>
       <c r="O324" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="325" spans="1:15" x14ac:dyDescent="0.2">
@@ -34187,7 +34291,7 @@
       <c r="J325" s="49"/>
       <c r="K325" s="49"/>
       <c r="O325" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="326" spans="1:15" x14ac:dyDescent="0.2">
@@ -34217,7 +34321,7 @@
       <c r="J326" s="49"/>
       <c r="K326" s="49"/>
       <c r="O326" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="327" spans="1:15" x14ac:dyDescent="0.2">
@@ -34247,7 +34351,7 @@
       <c r="J327" s="49"/>
       <c r="K327" s="49"/>
       <c r="O327" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="328" spans="1:15" x14ac:dyDescent="0.2">
@@ -34277,7 +34381,7 @@
       <c r="J328" s="49"/>
       <c r="K328" s="49"/>
       <c r="O328" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="329" spans="1:15" x14ac:dyDescent="0.2">
@@ -34307,7 +34411,7 @@
       <c r="J329" s="49"/>
       <c r="K329" s="49"/>
       <c r="O329" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="330" spans="1:15" x14ac:dyDescent="0.2">
@@ -34337,7 +34441,7 @@
       <c r="J330" s="49"/>
       <c r="K330" s="49"/>
       <c r="O330" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="331" spans="1:15" x14ac:dyDescent="0.2">
@@ -34367,7 +34471,7 @@
       <c r="J331" s="49"/>
       <c r="K331" s="49"/>
       <c r="O331" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="332" spans="1:15" x14ac:dyDescent="0.2">
@@ -34397,7 +34501,7 @@
       <c r="J332" s="49"/>
       <c r="K332" s="49"/>
       <c r="O332" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="333" spans="1:15" x14ac:dyDescent="0.2">
@@ -34427,7 +34531,7 @@
       <c r="J333" s="49"/>
       <c r="K333" s="49"/>
       <c r="O333" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="334" spans="1:15" x14ac:dyDescent="0.2">
@@ -34457,7 +34561,7 @@
       <c r="J334" s="49"/>
       <c r="K334" s="49"/>
       <c r="O334" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="335" spans="1:15" x14ac:dyDescent="0.2">
@@ -34487,7 +34591,7 @@
       <c r="J335" s="49"/>
       <c r="K335" s="49"/>
       <c r="O335" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="336" spans="1:15" x14ac:dyDescent="0.2">
@@ -34517,7 +34621,7 @@
       <c r="J336" s="49"/>
       <c r="K336" s="49"/>
       <c r="O336" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="337" spans="1:15" x14ac:dyDescent="0.2">
@@ -34547,7 +34651,7 @@
       <c r="J337" s="49"/>
       <c r="K337" s="49"/>
       <c r="O337" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="338" spans="1:15" x14ac:dyDescent="0.2">
@@ -34577,7 +34681,7 @@
       <c r="J338" s="49"/>
       <c r="K338" s="49"/>
       <c r="O338" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="339" spans="1:15" x14ac:dyDescent="0.2">
@@ -34607,7 +34711,7 @@
       <c r="J339" s="49"/>
       <c r="K339" s="49"/>
       <c r="O339" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="340" spans="1:15" x14ac:dyDescent="0.2">
@@ -34637,7 +34741,7 @@
       <c r="J340" s="49"/>
       <c r="K340" s="49"/>
       <c r="O340" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="341" spans="1:15" x14ac:dyDescent="0.2">
@@ -34667,7 +34771,7 @@
       <c r="J341" s="49"/>
       <c r="K341" s="49"/>
       <c r="O341" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
     <row r="342" spans="1:15" x14ac:dyDescent="0.2">
@@ -34697,7 +34801,7 @@
       <c r="J342" s="49"/>
       <c r="K342" s="49"/>
       <c r="O342" s="49" t="s">
-        <v>424</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -34751,10 +34855,10 @@
         <v>10</v>
       </c>
       <c r="E1" s="55" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="F1" s="55" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G1" s="55" t="s">
         <v>11</v>
@@ -35244,7 +35348,7 @@
         <v>85</v>
       </c>
       <c r="D19" s="48" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="E19" s="48"/>
       <c r="F19" s="48"/>
@@ -36728,7 +36832,7 @@
         <v>153</v>
       </c>
       <c r="D72" s="48" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E72" s="48"/>
       <c r="F72" s="48"/>
@@ -36876,7 +36980,7 @@
         <v>279727</v>
       </c>
       <c r="H77" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I77">
         <v>1</v>
@@ -36932,7 +37036,7 @@
         <v>124548</v>
       </c>
       <c r="H79" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I79">
         <v>0.98827384817519359</v>
@@ -37324,7 +37428,7 @@
         <v>130776</v>
       </c>
       <c r="H93" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I93">
         <v>0.95762172987052296</v>
@@ -37372,7 +37476,7 @@
         <v>183</v>
       </c>
       <c r="D95" s="48" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E95" s="48"/>
       <c r="F95" s="48"/>
@@ -37764,7 +37868,7 @@
         <v>183</v>
       </c>
       <c r="D109" s="48" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="E109" s="48"/>
       <c r="F109" s="48"/>
@@ -38268,7 +38372,7 @@
         <v>213</v>
       </c>
       <c r="D127" s="48" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E127" s="48"/>
       <c r="F127" s="48"/>
@@ -38324,7 +38428,7 @@
         <v>213</v>
       </c>
       <c r="D129" s="48" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E129" s="48"/>
       <c r="F129" s="48"/>
@@ -39724,7 +39828,7 @@
         <v>258</v>
       </c>
       <c r="D179" s="48" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="E179" s="48"/>
       <c r="F179" s="48"/>
@@ -39920,7 +40024,7 @@
         <v>258</v>
       </c>
       <c r="D186" s="48" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="E186" s="48"/>
       <c r="F186" s="48"/>
@@ -40340,7 +40444,7 @@
         <v>213</v>
       </c>
       <c r="D201" s="48" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="E201" s="48"/>
       <c r="F201" s="48"/>
@@ -40872,7 +40976,7 @@
         <v>296</v>
       </c>
       <c r="D220" s="48" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="E220" s="48"/>
       <c r="F220" s="48"/>
@@ -40984,7 +41088,7 @@
         <v>304</v>
       </c>
       <c r="D224" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="E224" s="48"/>
       <c r="F224" s="48"/>
@@ -41572,7 +41676,7 @@
         <v>320</v>
       </c>
       <c r="D245" s="48" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="E245" s="48"/>
       <c r="F245" s="48"/>
@@ -44352,10 +44456,10 @@
         <v>10</v>
       </c>
       <c r="E1" s="55" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="F1" s="55" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G1" s="55" t="s">
         <v>11</v>
@@ -44382,7 +44486,7 @@
       <c r="G2" s="56"/>
       <c r="H2" s="58"/>
       <c r="I2" s="46" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="J2" s="46" t="s">
         <v>30</v>
@@ -45051,7 +45155,7 @@
         <v>85</v>
       </c>
       <c r="D19" s="48" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="E19" s="48"/>
       <c r="F19" s="48"/>
@@ -47171,7 +47275,7 @@
         <v>153</v>
       </c>
       <c r="D72" s="48" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E72" s="48"/>
       <c r="F72" s="48"/>
@@ -47379,7 +47483,7 @@
         <v>279727</v>
       </c>
       <c r="H77" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I77" s="7" t="s">
         <v>4</v>
@@ -47459,7 +47563,7 @@
         <v>124548</v>
       </c>
       <c r="H79" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I79" s="7" t="s">
         <v>4</v>
@@ -48019,7 +48123,7 @@
         <v>130776</v>
       </c>
       <c r="H93" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I93" s="7" t="s">
         <v>4</v>
@@ -48091,7 +48195,7 @@
         <v>183</v>
       </c>
       <c r="D95" s="48" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E95" s="48"/>
       <c r="F95" s="48"/>
@@ -48651,7 +48755,7 @@
         <v>183</v>
       </c>
       <c r="D109" s="48" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="E109" s="48"/>
       <c r="F109" s="48"/>
@@ -49371,7 +49475,7 @@
         <v>213</v>
       </c>
       <c r="D127" s="48" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E127" s="48"/>
       <c r="F127" s="48"/>
@@ -49451,7 +49555,7 @@
         <v>213</v>
       </c>
       <c r="D129" s="48" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E129" s="48"/>
       <c r="F129" s="48"/>
@@ -51451,7 +51555,7 @@
         <v>258</v>
       </c>
       <c r="D179" s="48" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="E179" s="48"/>
       <c r="F179" s="48"/>
@@ -51731,7 +51835,7 @@
         <v>258</v>
       </c>
       <c r="D186" s="48" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="E186" s="48"/>
       <c r="F186" s="48"/>
@@ -52331,7 +52435,7 @@
         <v>213</v>
       </c>
       <c r="D201" s="48" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="E201" s="48"/>
       <c r="F201" s="48"/>
@@ -53091,7 +53195,7 @@
         <v>296</v>
       </c>
       <c r="D220" s="48" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="E220" s="48"/>
       <c r="F220" s="48"/>
@@ -53251,7 +53355,7 @@
         <v>304</v>
       </c>
       <c r="D224" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="E224" s="48"/>
       <c r="F224" s="48"/>
@@ -54091,7 +54195,7 @@
         <v>320</v>
       </c>
       <c r="D245" s="48" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="E245" s="48"/>
       <c r="F245" s="48"/>
@@ -58102,10 +58206,10 @@
     <row r="6" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="75"/>
       <c r="B6" s="39" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>44</v>
@@ -58118,7 +58222,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>44</v>
@@ -58455,7 +58559,7 @@
         <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: added total POB
</commit_message>
<xml_diff>
--- a/src/Data/country_data.xlsx
+++ b/src/Data/country_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC335E5B-C45F-0D47-89B0-BD66DBC5AFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F62E5A-066E-DB44-AC30-F108ABC2822A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45980" yWindow="2780" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{7CFA64C4-648F-B840-901A-EC2D94882293}"/>
+    <workbookView xWindow="45980" yWindow="2780" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{7CFA64C4-648F-B840-901A-EC2D94882293}"/>
   </bookViews>
   <sheets>
     <sheet name="1-General" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7657" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7658" uniqueCount="449">
   <si>
     <t>Datos generales</t>
   </si>
@@ -1390,6 +1390,9 @@
   <si>
     <t>Na</t>
   </si>
+  <si>
+    <t>Población total</t>
+  </si>
 </sst>
 </file>
 
@@ -2557,9 +2560,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD1E9FE-E77B-E547-ADE0-516025CB78C4}">
-  <dimension ref="A1:G341"/>
+  <dimension ref="A1:H341"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2570,9 +2575,10 @@
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>7</v>
       </c>
@@ -2594,8 +2600,11 @@
       <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>16</v>
       </c>
@@ -2613,8 +2622,9 @@
       <c r="G2" s="47">
         <v>25227</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="47"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>16</v>
       </c>
@@ -2632,8 +2642,9 @@
       <c r="G3" s="47">
         <v>10813</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="47"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>16</v>
       </c>
@@ -2651,8 +2662,9 @@
       <c r="G4" s="47">
         <v>42579</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="47"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>16</v>
       </c>
@@ -2670,8 +2682,9 @@
       <c r="G5" s="47">
         <v>77422</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="47"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>16</v>
       </c>
@@ -2689,8 +2702,9 @@
       <c r="G6" s="47">
         <v>29805</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="47"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>16</v>
       </c>
@@ -2708,8 +2722,9 @@
       <c r="G7" s="47">
         <v>9546</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="47"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>16</v>
       </c>
@@ -2728,7 +2743,7 @@
         <v>17348</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>16</v>
       </c>
@@ -2747,7 +2762,7 @@
         <v>32877</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>16</v>
       </c>
@@ -2766,7 +2781,7 @@
         <v>15361</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>16</v>
       </c>
@@ -2785,7 +2800,7 @@
         <v>30608</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>16</v>
       </c>
@@ -2804,7 +2819,7 @@
         <v>21737</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>16</v>
       </c>
@@ -2823,7 +2838,7 @@
         <v>92351</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>16</v>
       </c>
@@ -2842,7 +2857,7 @@
         <v>12986</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>16</v>
       </c>
@@ -2861,7 +2876,7 @@
         <v>37630</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
@@ -23791,7 +23806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24FC60A-8114-B04C-B5D4-941061AFF1F9}">
   <dimension ref="A1:O342"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
refactor: update el polio for la polio
</commit_message>
<xml_diff>
--- a/src/Data/country_data.xlsx
+++ b/src/Data/country_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F62E5A-066E-DB44-AC30-F108ABC2822A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF1F690-B9A5-3846-8C6A-8E76ACDFA38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45980" yWindow="2780" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{7CFA64C4-648F-B840-901A-EC2D94882293}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7CFA64C4-648F-B840-901A-EC2D94882293}"/>
   </bookViews>
   <sheets>
     <sheet name="1-General" sheetId="1" r:id="rId1"/>
@@ -1385,13 +1385,13 @@
     <t>Número total de municipios</t>
   </si>
   <si>
-    <t>Esquema de vacunación contra el polio</t>
-  </si>
-  <si>
     <t>Na</t>
   </si>
   <si>
     <t>Población total</t>
+  </si>
+  <si>
+    <t>Esquema de vacunación contra la polio</t>
   </si>
 </sst>
 </file>
@@ -2493,8 +2493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18904028-F9F6-3046-9356-B730934F1CDF}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2544,7 +2544,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B6" s="2"/>
     </row>
@@ -2562,7 +2562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD1E9FE-E77B-E547-ADE0-516025CB78C4}">
   <dimension ref="A1:H341"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -2601,7 +2601,7 @@
         <v>11</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -23932,7 +23932,7 @@
         <v>0</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -58441,7 +58441,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="97" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="29" t="s">
         <v>28</v>
@@ -58510,7 +58510,7 @@
       </c>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="72"/>
       <c r="B26" s="29" t="s">
         <v>79</v>

</xml_diff>